<commit_message>
Refactor DNN model and training pipeline
</commit_message>
<xml_diff>
--- a/计算结果.xlsx
+++ b/计算结果.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27602"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29803"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://76rp4l-my.sharepoint.com/personal/nothingnessvoid_76rp4l_onmicrosoft_com/Documents/学校用/毕业设计/Graduation-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://76rp4l-my.sharepoint.com/personal/nothingnessvoid_76rp4l_onmicrosoft_com/Documents/学校用/毕业用/Graduation-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_4831E4391B66560F62355476585DCE3A87402652" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B121961-FD04-4CA9-943A-B11B55EF0F6F}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_4831E4391B66560F62355476585DCE3A87402652" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E7C9035-9511-446F-9865-FBCF78066BB0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,13 +479,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1:AD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +578,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>90.031694052000006</v>
       </c>
@@ -663,7 +667,7 @@
         <v>4.2940558215578663E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>86.036779432000003</v>
       </c>
@@ -752,7 +756,7 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>86.036779432000003</v>
       </c>
@@ -841,7 +845,7 @@
         <v>-0.45</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>18.010564683999998</v>
       </c>
@@ -930,7 +934,7 @@
         <v>0.46459835653194698</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>84.003371127999998</v>
       </c>
@@ -1019,7 +1023,7 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>168.09727151199999</v>
       </c>
@@ -1108,7 +1112,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>196.12857163999999</v>
       </c>
@@ -1197,7 +1201,7 @@
         <v>-1.06</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>252.19117189599999</v>
       </c>
@@ -1286,7 +1290,7 @@
         <v>-0.38</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>104.062600256</v>
       </c>
@@ -1375,7 +1379,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>44.026214748000001</v>
       </c>
@@ -1464,7 +1468,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>54.046950191999997</v>
       </c>
@@ -1553,7 +1557,7 @@
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>54.046950191999997</v>
       </c>
@@ -1642,7 +1646,7 @@
         <v>0.40300000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>54.046950191999997</v>
       </c>
@@ -1731,7 +1735,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>54.046950191999997</v>
       </c>
@@ -1820,7 +1824,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>54.046950191999997</v>
       </c>
@@ -1909,7 +1913,7 @@
         <v>0.41099999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>54.046950191999997</v>
       </c>
@@ -1998,7 +2002,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>68.062600255999996</v>
       </c>
@@ -2087,7 +2091,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>68.062600255999996</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>0.373</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>68.062600255999996</v>
       </c>
@@ -2265,7 +2269,7 @@
         <v>0.39500000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>68.062600255999996</v>
       </c>
@@ -2354,7 +2358,7 @@
         <v>0.437</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>68.062600255999996</v>
       </c>
@@ -2443,7 +2447,7 @@
         <v>0.438</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>68.062600255999996</v>
       </c>
@@ -2532,7 +2536,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>160.12520051199999</v>
       </c>
@@ -2621,7 +2625,7 @@
         <v>0.10683287570931729</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>160.12520051199999</v>
       </c>
@@ -2710,7 +2714,7 @@
         <v>8.3494971375522212E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>160.12520051199999</v>
       </c>
@@ -2799,7 +2803,7 @@
         <v>7.4339796064914573E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>160.12520051199999</v>
       </c>
@@ -2888,7 +2892,7 @@
         <v>6.6411362722765654E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>104.062600256</v>
       </c>
@@ -2977,7 +2981,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>72.021129368000004</v>
       </c>
@@ -3066,7 +3070,7 @@
         <v>0.505</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>72.057514875999999</v>
       </c>
@@ -3155,7 +3159,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>117.91438307200001</v>
       </c>
@@ -3244,7 +3248,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>72.057514875999999</v>
       </c>
@@ -3333,7 +3337,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>117.91438307200001</v>
       </c>
@@ -3422,7 +3426,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>104.062600256</v>
       </c>
@@ -3511,7 +3515,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>176.10212704200001</v>
       </c>
@@ -3600,7 +3604,7 @@
         <v>0.46206104309911122</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>104.062600256</v>
       </c>
@@ -3689,7 +3693,7 @@
         <v>2.7846629553430959E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>104.062600256</v>
       </c>
@@ -3778,7 +3782,7 @@
         <v>1.5540658682634729</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>110.10955044799999</v>
       </c>
@@ -3867,7 +3871,7 @@
         <v>0.36664726340838372</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>110.10955044799999</v>
       </c>
@@ -3956,7 +3960,7 @@
         <v>0.28485130744236431</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>110.10955044799999</v>
       </c>
@@ -4045,7 +4049,7 @@
         <v>0.2527637512566423</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>110.10955044799999</v>
       </c>
@@ -4134,7 +4138,7 @@
         <v>0.22497574701862519</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>100.052429496</v>
       </c>
@@ -4223,7 +4227,7 @@
         <v>1.4990000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>116.047344116</v>
       </c>
@@ -4312,7 +4316,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>116.047344116</v>
       </c>
@@ -4401,7 +4405,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>86.036779432000003</v>
       </c>
@@ -4490,7 +4494,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>142.099379688</v>
       </c>
@@ -4579,7 +4583,7 @@
         <v>0.59406447211325264</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>142.099379688</v>
       </c>
@@ -4668,7 +4672,7 @@
         <v>0.50686849735630224</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>142.099379688</v>
       </c>
@@ -4757,7 +4761,7 @@
         <v>0.53322360566263005</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>142.099379688</v>
       </c>
@@ -4846,7 +4850,7 @@
         <v>0.56172778441071125</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>72.057514875999999</v>
       </c>
@@ -4935,7 +4939,7 @@
         <v>-2.2500000000000001E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>72.057514875999999</v>
       </c>
@@ -5024,7 +5028,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>44.026214748000001</v>
       </c>
@@ -5113,7 +5117,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>44.026214748000001</v>
       </c>
@@ -5202,7 +5206,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>104.062600256</v>
       </c>
@@ -5291,7 +5295,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>104.062600256</v>
       </c>
@@ -5380,7 +5384,7 @@
         <v>0.26157894736842102</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>104.062600256</v>
       </c>
@@ -5469,7 +5473,7 @@
         <v>0.1633333333333333</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>104.062600256</v>
       </c>
@@ -5558,7 +5562,7 @@
         <v>0.13322580645161289</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>104.062600256</v>
       </c>
@@ -5647,7 +5651,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>128.083729624</v>
       </c>
@@ -5736,7 +5740,7 @@
         <v>3.441427155599603E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>128.083729624</v>
       </c>
@@ -5825,7 +5829,7 @@
         <v>3.4575607274577133E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>128.083729624</v>
       </c>
@@ -5914,7 +5918,7 @@
         <v>3.4816442988481452E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>128.083729624</v>
       </c>
@@ -6003,7 +6007,7 @@
         <v>3.4908701159505007E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>90.031694052000006</v>
       </c>
@@ -6092,7 +6096,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>222.08920892800001</v>
       </c>
@@ -6181,7 +6185,7 @@
         <v>2.1340106168771742</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>222.08920892800001</v>
       </c>
@@ -6270,7 +6274,7 @@
         <v>1.6026767754912581</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>222.08920892800001</v>
       </c>
@@ -6359,7 +6363,7 @@
         <v>1.394240988079851</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>222.08920892800001</v>
       </c>
@@ -6448,7 +6452,7 @@
         <v>1.213734423154228</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>278.15180918400063</v>
       </c>
@@ -6537,7 +6541,7 @@
         <v>1.1533443163097199</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>278.15180918400063</v>
       </c>
@@ -6626,7 +6630,7 @@
         <v>0.88824384960544633</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>278.15180918400063</v>
       </c>
@@ -6715,7 +6719,7 @@
         <v>0.78424816889271876</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>278.15180918400063</v>
       </c>
@@ -6804,7 +6808,7 @@
         <v>0.69418732413238637</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>104.062600256</v>
       </c>
@@ -6893,7 +6897,7 @@
         <v>-0.1319213984989932</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>104.062600256</v>
       </c>
@@ -6982,7 +6986,7 @@
         <v>-0.13196450564753209</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>104.062600256</v>
       </c>
@@ -7071,7 +7075,7 @@
         <v>-0.1319814160562976</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>104.062600256</v>
       </c>
@@ -7160,7 +7164,7 @@
         <v>-0.13199606056545629</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>104.062600256</v>
       </c>
@@ -7249,7 +7253,7 @@
         <v>5.7312374153395573E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>104.062600256</v>
       </c>
@@ -7338,7 +7342,7 @@
         <v>5.5020501315178723E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>104.062600256</v>
       </c>
@@ -7427,7 +7431,7 @@
         <v>5.4121427545598157E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>104.062600256</v>
       </c>
@@ -7516,7 +7520,7 @@
         <v>5.3342824601366752E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>99.068413907999997</v>
       </c>
@@ -7605,7 +7609,7 @@
         <v>0.27491467989834212</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>168.09727151199999</v>
       </c>
@@ -7694,7 +7698,7 @@
         <v>0.15691483422352109</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>168.09727151199999</v>
       </c>
@@ -7783,7 +7787,7 @@
         <v>0.1565155051215103</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>168.09727151199999</v>
       </c>
@@ -7872,7 +7876,7 @@
         <v>0.15572520941364179</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>168.09727151199999</v>
       </c>
@@ -7961,7 +7965,7 @@
         <v>0.15533418463678819</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>252.19117189599999</v>
       </c>
@@ -8050,7 +8054,7 @@
         <v>0.15798659261424541</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>252.19117189599999</v>
       </c>
@@ -8139,7 +8143,7 @@
         <v>0.1576220692330069</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>252.19117189599999</v>
       </c>
@@ -8228,7 +8232,7 @@
         <v>0.1569035244406031</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>252.19117189599999</v>
       </c>
@@ -8317,7 +8321,7 @@
         <v>0.15654940265698181</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>189.15174960799999</v>
       </c>
@@ -8406,7 +8410,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>99.068413907999997</v>
       </c>
@@ -8495,7 +8499,7 @@
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>99.068413907999997</v>
       </c>
@@ -8584,7 +8588,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>64.012456503999999</v>
       </c>
@@ -8673,7 +8677,7 @@
         <v>-0.29499999999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>104.062600256</v>
       </c>
@@ -8762,7 +8766,7 @@
         <v>-0.11498151198974919</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>104.062600256</v>
       </c>
@@ -8851,7 +8855,7 @@
         <v>-7.9861364691319839E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>104.062600256</v>
       </c>
@@ -8940,7 +8944,7 @@
         <v>-6.6084159126813161E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>104.062600256</v>
       </c>
@@ -9029,7 +9033,7 @@
         <v>-5.4153021573093943E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>104.062600256</v>
       </c>
@@ -9118,7 +9122,7 @@
         <v>3.8892307692307691E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>104.062600256</v>
       </c>
@@ -9207,7 +9211,7 @@
         <v>3.2417391304347822E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>104.062600256</v>
       </c>
@@ -9296,7 +9300,7 @@
         <v>2.2586861313868611E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>104.062600256</v>
       </c>
@@ -9385,7 +9389,7 @@
         <v>1.8767567567567572E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>104.062600256</v>
       </c>
@@ -9474,7 +9478,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>68.062600255999996</v>
       </c>
@@ -9563,7 +9567,7 @@
         <v>0.17466410256410261</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>68.062600255999996</v>
       </c>
@@ -9652,7 +9656,7 @@
         <v>0.15241884057971011</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>68.062600255999996</v>
       </c>
@@ -9741,7 +9745,7 @@
         <v>0.11864501216545011</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>68.062600255999996</v>
       </c>
@@ -9830,7 +9834,7 @@
         <v>0.1055234234234234</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>104.062600256</v>
       </c>
@@ -9919,7 +9923,7 @@
         <v>5.3510256410256397E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>104.062600256</v>
       </c>
@@ -10008,7 +10012,7 @@
         <v>4.6201449275362322E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>104.062600256</v>
       </c>
@@ -10097,7 +10101,7 @@
         <v>3.5104866180048669E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>104.062600256</v>
       </c>
@@ -10186,7 +10190,7 @@
         <v>3.079369369369369E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>104.062600256</v>
       </c>
@@ -10275,7 +10279,7 @@
         <v>0.35608768076148639</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>104.062600256</v>
       </c>
@@ -10364,7 +10368,7 @@
         <v>0.26834395791428128</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>104.062600256</v>
       </c>
@@ -10453,7 +10457,7 @@
         <v>0.23392316530231219</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>104.062600256</v>
       </c>
@@ -10542,7 +10546,7 @@
         <v>0.2041145651882621</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>104.062600256</v>
       </c>
@@ -10631,7 +10635,7 @@
         <v>0.1453646348160352</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>104.062600256</v>
       </c>
@@ -10720,7 +10724,7 @@
         <v>0.1118872040847904</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>104.062600256</v>
       </c>
@@ -10809,7 +10813,7 @@
         <v>9.8754416199913861E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A117">
         <v>104.062600256</v>
       </c>
@@ -10898,7 +10902,7 @@
         <v>8.7381347983384719E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A118">
         <v>104.062600256</v>
       </c>
@@ -10987,7 +10991,7 @@
         <v>3.4813472451034229E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A119">
         <v>104.062600256</v>
       </c>
@@ -11076,7 +11080,7 @@
         <v>3.2830883490639021E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A120">
         <v>104.062600256</v>
       </c>
@@ -11165,7 +11169,7 @@
         <v>3.2053138015223318E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A121">
         <v>104.062600256</v>
       </c>
@@ -11254,7 +11258,7 @@
         <v>3.1379606056545627E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A122">
         <v>42.046950191999997</v>
       </c>
@@ -11343,7 +11347,7 @@
         <v>0.39400000000000002</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A123">
         <v>104.062600256</v>
       </c>
@@ -11432,7 +11436,7 @@
         <v>0.1170297638660077</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A124">
         <v>104.062600256</v>
       </c>
@@ -11521,7 +11525,7 @@
         <v>0.1000361442054773</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A125">
         <v>104.062600256</v>
       </c>
@@ -11610,7 +11614,7 @@
         <v>9.3369754416199921E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A126">
         <v>104.062600256</v>
       </c>
@@ -11699,7 +11703,7 @@
         <v>8.759662334181964E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A127">
         <v>100.052429496</v>
       </c>
@@ -11788,7 +11792,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A128">
         <v>104.062600256</v>
       </c>
@@ -11877,7 +11881,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A129">
         <v>58.041864812</v>
       </c>
@@ -11966,7 +11970,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A130">
         <v>58.041864812</v>
       </c>
@@ -12055,7 +12059,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A131">
         <v>92.062600255999996</v>
       </c>
@@ -12144,7 +12148,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A132">
         <v>92.062600255999996</v>
       </c>
@@ -12233,7 +12237,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A133">
         <v>75.944141999999999</v>
       </c>
@@ -12322,7 +12326,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A134">
         <v>75.944141999999999</v>
       </c>
@@ -12411,7 +12415,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A135">
         <v>104.062600256</v>
       </c>
@@ -12500,7 +12504,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A136">
         <v>100.052429496</v>
       </c>
@@ -12589,7 +12593,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A137">
         <v>68.062600255999996</v>
       </c>
@@ -12678,7 +12682,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A138">
         <v>104.062600256</v>
       </c>
@@ -12767,7 +12771,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A139">
         <v>117.91438307200001</v>
       </c>
@@ -12856,7 +12860,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A140">
         <v>72.021129368000004</v>
       </c>
@@ -12945,7 +12949,7 @@
         <v>1.0569999999999999</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A141">
         <v>128.083729624</v>
       </c>
@@ -13034,7 +13038,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A142">
         <v>168.039814124</v>
       </c>
@@ -13123,7 +13127,7 @@
         <v>0.54200000000000004</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A143">
         <v>104.062600256</v>
       </c>
@@ -13212,7 +13216,7 @@
         <v>-1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A144">
         <v>104.062600256</v>
       </c>
@@ -13301,7 +13305,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A145">
         <v>68.062600255999996</v>
       </c>
@@ -13390,7 +13394,7 @@
         <v>0.12645641588870579</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A146">
         <v>68.062600255999996</v>
       </c>
@@ -13479,7 +13483,7 @@
         <v>9.8813461240909811E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A147">
         <v>68.062600255999996</v>
       </c>
@@ -13568,7 +13572,7 @@
         <v>8.7969467183685202E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A148">
         <v>68.062600255999996</v>
       </c>
@@ -13657,7 +13661,7 @@
         <v>7.8578507302693279E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A149">
         <v>104.062600256</v>
       </c>
@@ -13746,7 +13750,7 @@
         <v>3.2715174812374147E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A150">
         <v>104.062600256</v>
       </c>
@@ -13835,7 +13839,7 @@
         <v>3.0902522048584249E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A151">
         <v>104.062600256</v>
       </c>
@@ -13924,7 +13928,7 @@
         <v>3.0191440471061329E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A152">
         <v>104.062600256</v>
       </c>
@@ -14013,7 +14017,7 @@
         <v>2.9575639823127432E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A153">
         <v>104.062600256</v>
       </c>
@@ -14102,7 +14106,7 @@
         <v>0.17333333333333331</v>
       </c>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A154">
         <v>104.062600256</v>
       </c>
@@ -14191,7 +14195,7 @@
         <v>0.2471433278418452</v>
       </c>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A155">
         <v>104.062600256</v>
       </c>
@@ -14280,7 +14284,7 @@
         <v>0.19157419155191091</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A156">
         <v>104.062600256</v>
       </c>
@@ -14369,7 +14373,7 @@
         <v>0.16977509694097381</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A157">
         <v>104.062600256</v>
       </c>
@@ -14458,7 +14462,7 @@
         <v>0.15089695832775021</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A158">
         <v>104.062600256</v>
       </c>
@@ -14547,7 +14551,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A159">
         <v>104.062600256</v>
       </c>
@@ -14636,7 +14640,7 @@
         <v>-3.0000000000000031E-3</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A160">
         <v>105.05784922399999</v>
       </c>
@@ -14725,7 +14729,7 @@
         <v>-3.999999999999998E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A161">
         <v>104.062600256</v>
       </c>
@@ -14814,7 +14818,7 @@
         <v>4.2277869302580998E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A162">
         <v>104.062600256</v>
       </c>
@@ -14903,7 +14907,7 @@
         <v>4.0068698746712053E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A163">
         <v>104.062600256</v>
       </c>
@@ -14992,7 +14996,7 @@
         <v>3.9202068074105992E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A164">
         <v>104.062600256</v>
       </c>
@@ -15081,7 +15085,7 @@
         <v>3.8451561034436553E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A165">
         <v>160.12520051199999</v>
       </c>
@@ -15170,7 +15174,7 @@
         <v>0.11739224978403059</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A166">
         <v>160.12520051199999</v>
       </c>
@@ -15259,7 +15263,7 @@
         <v>0.1069213698947125</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A167">
         <v>160.12520051199999</v>
       </c>
@@ -15348,7 +15352,7 @@
         <v>8.9468826493880521E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A168">
         <v>160.12520051199999</v>
       </c>
@@ -15437,7 +15441,7 @@
         <v>8.2119984410016583E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A169">
         <v>104.062600256</v>
       </c>
@@ -15526,7 +15530,7 @@
         <v>0.1976425041186162</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A170">
         <v>104.062600256</v>
       </c>
@@ -15615,7 +15619,7 @@
         <v>0.16195590283150241</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A171">
         <v>104.062600256</v>
       </c>
@@ -15704,7 +15708,7 @@
         <v>0.14795648427401981</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A172">
         <v>104.062600256</v>
       </c>
@@ -15793,7 +15797,7 @@
         <v>0.1358329090178213</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A173">
         <v>18.010564683999998</v>
       </c>
@@ -15882,7 +15886,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A174">
         <v>18.010564683999998</v>
       </c>
@@ -15971,7 +15975,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A175">
         <v>104.062600256</v>
       </c>
@@ -16060,7 +16064,7 @@
         <v>0.19700000000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A176">
         <v>104.062600256</v>
       </c>
@@ -16149,7 +16153,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A177">
         <v>32.026214748000001</v>
       </c>
@@ -16238,7 +16242,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A178">
         <v>18.010564683999998</v>
       </c>
@@ -16327,7 +16331,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A179">
         <v>104.062600256</v>
       </c>
@@ -16416,7 +16420,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A180">
         <v>104.062600256</v>
       </c>
@@ -16505,7 +16509,7 @@
         <v>0.2403468790042102</v>
       </c>
     </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A181">
         <v>104.062600256</v>
       </c>
@@ -16594,7 +16598,7 @@
         <v>0.1884596936407241</v>
       </c>
     </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A182">
         <v>104.062600256</v>
       </c>
@@ -16683,7 +16687,7 @@
         <v>0.16810498348413039</v>
       </c>
     </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A183">
         <v>104.062600256</v>
       </c>
@@ -16772,7 +16776,7 @@
         <v>0.15047768993702271</v>
       </c>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A184">
         <v>104.062600256</v>
       </c>
@@ -16861,7 +16865,7 @@
         <v>4.0871242906827747E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A185">
         <v>104.062600256</v>
       </c>
@@ -16950,7 +16954,7 @@
         <v>3.9065387590902063E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A186">
         <v>104.062600256</v>
       </c>
@@ -17039,7 +17043,7 @@
         <v>3.8356972569294837E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A187">
         <v>104.062600256</v>
       </c>
@@ -17128,7 +17132,7 @@
         <v>3.7743481173790699E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A188">
         <v>104.062600256</v>
       </c>
@@ -17217,7 +17221,7 @@
         <v>3.2715174812374147E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A189">
         <v>104.062600256</v>
       </c>
@@ -17306,7 +17310,7 @@
         <v>3.0902522048584249E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A190">
         <v>104.062600256</v>
       </c>
@@ -17395,7 +17399,7 @@
         <v>3.0191440471061329E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A191">
         <v>104.062600256</v>
       </c>
@@ -17484,7 +17488,7 @@
         <v>2.9575639823127432E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A192">
         <v>90.031694052000006</v>
       </c>
@@ -17573,7 +17577,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A193">
         <v>94.078250319999995</v>
       </c>
@@ -17662,7 +17666,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A194">
         <v>90.031694052000006</v>
       </c>
@@ -17751,7 +17755,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A195">
         <v>104.062600256</v>
       </c>
@@ -17840,7 +17844,7 @@
         <v>0.17569483800109839</v>
       </c>
     </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A196">
         <v>104.062600256</v>
       </c>
@@ -17929,7 +17933,7 @@
         <v>0.13525002320903609</v>
       </c>
     </row>
-    <row r="197" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A197">
         <v>104.062600256</v>
       </c>
@@ -18018,7 +18022,7 @@
         <v>0.1193840155105558</v>
       </c>
     </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A198">
         <v>104.062600256</v>
       </c>
@@ -18107,7 +18111,7 @@
         <v>0.1056439635535308</v>
       </c>
     </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A199">
         <v>104.062600256</v>
       </c>
@@ -18196,7 +18200,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="200" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A200">
         <v>68.062600255999996</v>
       </c>
@@ -18285,7 +18289,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A201">
         <v>104.062600256</v>
       </c>
@@ -18374,7 +18378,7 @@
         <v>-4.9999999999999989E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A202">
         <v>104.062600256</v>
       </c>
@@ -18463,7 +18467,7 @@
         <v>3.04E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A203">
         <v>104.062600256</v>
       </c>
@@ -18552,7 +18556,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A204">
         <v>104.062600256</v>
       </c>
@@ -18641,7 +18645,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="205" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A205">
         <v>104.062600256</v>
       </c>
@@ -18730,7 +18734,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="206" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A206">
         <v>104.062600256</v>
       </c>
@@ -18819,7 +18823,7 @@
         <v>-2.9999999999999992E-3</v>
       </c>
     </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A207">
         <v>104.062600256</v>
       </c>
@@ -18908,7 +18912,7 @@
         <v>7.2201319787662477E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A208">
         <v>104.062600256</v>
       </c>
@@ -18997,7 +19001,7 @@
         <v>5.5130095930682348E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A209">
         <v>104.062600256</v>
       </c>
@@ -19086,7 +19090,7 @@
         <v>4.8433262961367241E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A210">
         <v>104.062600256</v>
       </c>
@@ -19175,7 +19179,7 @@
         <v>4.2633767921747293E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A211">
         <v>170.130679816</v>
       </c>
@@ -19264,7 +19268,7 @@
         <v>-3.5000000000000009E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A212">
         <v>110.10955044799999</v>
       </c>
@@ -19353,7 +19357,7 @@
         <v>9.0233168588687546E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A213">
         <v>110.10955044799999</v>
       </c>
@@ -19442,7 +19446,7 @@
         <v>7.3579421321367786E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A214">
         <v>110.10955044799999</v>
       </c>
@@ -19531,7 +19535,7 @@
         <v>6.7046359327875921E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A215">
         <v>110.10955044799999</v>
       </c>
@@ -19620,7 +19624,7 @@
         <v>6.1388690874983248E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A216">
         <v>104.062600256</v>
       </c>
@@ -19709,7 +19713,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="217" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A217">
         <v>104.062600256</v>
       </c>
@@ -19798,7 +19802,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A218">
         <v>100.052429496</v>
       </c>
@@ -19887,7 +19891,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="219" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A219">
         <v>100.052429496</v>
       </c>
@@ -19976,7 +19980,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="220" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A220">
         <v>176.10212704200001</v>
       </c>
@@ -20065,7 +20069,7 @@
         <v>0.47780889621087308</v>
       </c>
     </row>
-    <row r="221" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A221">
         <v>176.10212704200001</v>
       </c>
@@ -20154,7 +20158,7 @@
         <v>0.44874980659136621</v>
       </c>
     </row>
-    <row r="222" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A222">
         <v>176.10212704200001</v>
       </c>
@@ -20243,7 +20247,7 @@
         <v>0.43735028005170179</v>
       </c>
     </row>
-    <row r="223" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A223">
         <v>176.10212704200001</v>
       </c>
@@ -20332,7 +20336,7 @@
         <v>0.42747822591451162</v>
       </c>
     </row>
-    <row r="224" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A224">
         <v>104.062600256</v>
       </c>
@@ -20421,7 +20425,7 @@
         <v>8.6097565440234308E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A225">
         <v>104.062600256</v>
       </c>
@@ -20510,7 +20514,7 @@
         <v>6.9217236577440833E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A226">
         <v>104.062600256</v>
       </c>
@@ -20599,7 +20603,7 @@
         <v>6.2595289386758596E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A227">
         <v>104.062600256</v>
       </c>
@@ -20688,7 +20692,7 @@
         <v>5.6860645852874182E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A228">
         <v>104.062600256</v>
       </c>
@@ -20777,7 +20781,7 @@
         <v>4.4528024894746478E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A229">
         <v>104.062600256</v>
       </c>
@@ -20866,7 +20870,7 @@
         <v>4.2001640105214302E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A230">
         <v>104.062600256</v>
       </c>
@@ -20955,7 +20959,7 @@
         <v>4.101057015654172E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A231">
         <v>104.062600256</v>
       </c>
@@ -21044,7 +21048,7 @@
         <v>4.0152298003483862E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A232">
         <v>104.062600256</v>
       </c>
@@ -21133,7 +21137,7 @@
         <v>0.35608768076148639</v>
       </c>
     </row>
-    <row r="233" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A233">
         <v>104.062600256</v>
       </c>
@@ -21222,7 +21226,7 @@
         <v>0.26834395791428128</v>
       </c>
     </row>
-    <row r="234" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A234">
         <v>104.062600256</v>
       </c>
@@ -21311,7 +21315,7 @@
         <v>0.23392316530231219</v>
       </c>
     </row>
-    <row r="235" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A235">
         <v>104.062600256</v>
       </c>
@@ -21400,7 +21404,7 @@
         <v>0.2041145651882621</v>
       </c>
     </row>
-    <row r="236" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A236">
         <v>44.026214748000001</v>
       </c>
@@ -21489,7 +21493,7 @@
         <v>0.36296448837634998</v>
       </c>
     </row>
-    <row r="237" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A237">
         <v>44.026214748000001</v>
       </c>
@@ -21578,7 +21582,7 @@
         <v>0.32614497911186757</v>
       </c>
     </row>
-    <row r="238" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A238">
         <v>44.026214748000001</v>
       </c>
@@ -21667,7 +21671,7 @@
         <v>0.31170113456843318</v>
       </c>
     </row>
-    <row r="239" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A239">
         <v>44.026214748000001</v>
       </c>
@@ -21756,7 +21760,7 @@
         <v>0.29919268390727588</v>
       </c>
     </row>
-    <row r="240" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A240">
         <v>104.062600256</v>
       </c>
@@ -21845,7 +21849,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A241">
         <v>100.052429496</v>
       </c>
@@ -21934,7 +21938,7 @@
         <v>-7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A242">
         <v>104.062600256</v>
       </c>
@@ -22023,7 +22027,7 @@
         <v>-0.02</v>
       </c>
     </row>
-    <row r="243" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A243">
         <v>104.062600256</v>
       </c>
@@ -22112,7 +22116,7 @@
         <v>1.5709542375983889E-3</v>
       </c>
     </row>
-    <row r="244" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A244">
         <v>104.062600256</v>
       </c>
@@ -22201,7 +22205,7 @@
         <v>1.3001892310072719E-3</v>
       </c>
     </row>
-    <row r="245" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A245">
         <v>104.062600256</v>
       </c>
@@ -22290,7 +22294,7 @@
         <v>1.1939714203647849E-3</v>
       </c>
     </row>
-    <row r="246" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A246">
         <v>104.062600256</v>
       </c>
@@ -22379,7 +22383,7 @@
         <v>1.10198619857966E-3</v>
       </c>
     </row>
-    <row r="247" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A247">
         <v>104.062600256</v>
       </c>
@@ -22468,7 +22472,7 @@
         <v>6.7138422112392473E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A248">
         <v>104.062600256</v>
       </c>
@@ -22557,7 +22561,7 @@
         <v>5.4336561968126272E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A249">
         <v>104.062600256</v>
       </c>
@@ -22646,7 +22650,7 @@
         <v>4.9314548326870607E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A250">
         <v>104.062600256</v>
       </c>
@@ -22735,7 +22739,7 @@
         <v>4.4965456250837477E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A251">
         <v>104.062600256</v>
       </c>
@@ -22824,7 +22828,7 @@
         <v>5.3510256410256397E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A252">
         <v>104.062600256</v>
       </c>
@@ -22913,7 +22917,7 @@
         <v>4.6201449275362322E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A253">
         <v>104.062600256</v>
       </c>
@@ -23002,7 +23006,7 @@
         <v>3.5104866180048669E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A254">
         <v>104.062600256</v>
       </c>
@@ -23091,7 +23095,7 @@
         <v>3.079369369369369E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A255">
         <v>68.062600255999996</v>
       </c>
@@ -23180,7 +23184,7 @@
         <v>0.33995442064799558</v>
       </c>
     </row>
-    <row r="256" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A256">
         <v>68.062600255999996</v>
       </c>
@@ -23269,7 +23273,7 @@
         <v>0.30545737273711898</v>
       </c>
     </row>
-    <row r="257" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A257">
         <v>68.062600255999996</v>
       </c>
@@ -23358,7 +23362,7 @@
         <v>0.29192460146488591</v>
       </c>
     </row>
-    <row r="258" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A258">
         <v>68.062600255999996</v>
       </c>
@@ -23447,7 +23451,7 @@
         <v>0.28020514538389391</v>
       </c>
     </row>
-    <row r="259" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A259">
         <v>104.062600256</v>
       </c>
@@ -23536,7 +23540,7 @@
         <v>9.1483221476510071E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A260">
         <v>104.062600256</v>
       </c>
@@ -23625,7 +23629,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="261" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A261">
         <v>104.062600256</v>
       </c>
@@ -23714,7 +23718,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="262" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A262">
         <v>104.062600256</v>
       </c>
@@ -23803,7 +23807,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="263" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A263">
         <v>104.062600256</v>
       </c>
@@ -23892,7 +23896,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="264" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A264">
         <v>104.062600256</v>
       </c>
@@ -23981,7 +23985,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="265" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A265">
         <v>90.031694052000006</v>
       </c>
@@ -24070,7 +24074,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="266" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A266">
         <v>90.031694052000006</v>
       </c>
@@ -24159,7 +24163,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="267" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A267">
         <v>90.031694052000006</v>
       </c>
@@ -24248,7 +24252,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="268" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A268">
         <v>90.031694052000006</v>
       </c>
@@ -24337,7 +24341,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="269" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A269">
         <v>90.031694052000006</v>
       </c>
@@ -24426,7 +24430,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="270" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A270">
         <v>104.062600256</v>
       </c>
@@ -24515,7 +24519,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="271" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A271">
         <v>104.062600256</v>
       </c>
@@ -24604,7 +24608,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="272" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A272">
         <v>104.062600256</v>
       </c>
@@ -24693,7 +24697,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="273" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A273">
         <v>90.031694052000006</v>
       </c>
@@ -24782,7 +24786,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="274" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A274">
         <v>90.031694052000006</v>
       </c>
@@ -24871,7 +24875,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="275" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A275">
         <v>90.031694052000006</v>
       </c>
@@ -24960,7 +24964,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="276" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A276">
         <v>90.031694052000006</v>
       </c>
@@ -25049,7 +25053,7 @@
         <v>2.19</v>
       </c>
     </row>
-    <row r="277" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A277">
         <v>104.062600256</v>
       </c>
@@ -25138,7 +25142,7 @@
         <v>4.4290780141843983E-2</v>
       </c>
     </row>
-    <row r="278" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A278">
         <v>104.062600256</v>
       </c>
@@ -25227,7 +25231,7 @@
         <v>4.3947068867387598E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A279">
         <v>104.062600256</v>
       </c>
@@ -25316,7 +25320,7 @@
         <v>4.3330683624801282E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A280">
         <v>104.062600256</v>
       </c>
@@ -25405,7 +25409,7 @@
         <v>4.3053278688524592E-2</v>
       </c>
     </row>
-    <row r="281" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A281">
         <v>104.062600256</v>
       </c>
@@ -25494,7 +25498,7 @@
         <v>5.6379492952590163E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A282">
         <v>104.062600256</v>
       </c>
@@ -25583,7 +25587,7 @@
         <v>4.8675718706483059E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A283">
         <v>104.062600256</v>
       </c>
@@ -25672,7 +25676,7 @@
         <v>4.5653622002010633E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A284">
         <v>104.062600256</v>
       </c>
@@ -25761,7 +25765,7 @@
         <v>4.3036469248291569E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A285">
         <v>104.062600256</v>
       </c>
@@ -25850,7 +25854,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="286" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A286">
         <v>104.062600256</v>
       </c>
@@ -25939,7 +25943,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A287">
         <v>114.06807956</v>
       </c>
@@ -26028,7 +26032,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A288">
         <v>104.062600256</v>
       </c>
@@ -26117,7 +26121,7 @@
         <v>-9.9999999999999742E-4</v>
       </c>
     </row>
-    <row r="289" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A289">
         <v>104.062600256</v>
       </c>
@@ -26206,7 +26210,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="290" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A290">
         <v>54.046950191999997</v>
       </c>
@@ -26295,7 +26299,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="291" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A291">
         <v>258.19836545200008</v>
       </c>
@@ -26384,7 +26388,7 @@
         <v>3.6402526084568933E-2</v>
       </c>
     </row>
-    <row r="292" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A292">
         <v>258.19836545200008</v>
       </c>
@@ -26473,7 +26477,7 @@
         <v>1.6689927278353708E-2</v>
       </c>
     </row>
-    <row r="293" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A293">
         <v>258.19836545200008</v>
       </c>
@@ -26562,7 +26566,7 @@
         <v>8.9569151227918975E-3</v>
       </c>
     </row>
-    <row r="294" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A294">
         <v>258.19836545200008</v>
       </c>
@@ -26651,7 +26655,7 @@
         <v>2.2600830765107942E-3</v>
       </c>
     </row>
-    <row r="295" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A295">
         <v>104.062600256</v>
       </c>
@@ -26740,7 +26744,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="296" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A296">
         <v>104.062600256</v>
       </c>
@@ -26829,7 +26833,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="297" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A297">
         <v>105.05784922399999</v>
       </c>
@@ -26918,7 +26922,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="298" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A298">
         <v>105.05784922399999</v>
       </c>
@@ -27007,7 +27011,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="299" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A299">
         <v>151.87541071999999</v>
       </c>
@@ -27096,7 +27100,7 @@
         <v>0.39600000000000002</v>
       </c>
     </row>
-    <row r="300" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A300">
         <v>84.093900383999994</v>
       </c>
@@ -27185,7 +27189,7 @@
         <v>0.505</v>
       </c>
     </row>
-    <row r="301" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A301">
         <v>104.062600256</v>
       </c>
@@ -27274,7 +27278,7 @@
         <v>0.438</v>
       </c>
     </row>
-    <row r="302" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A302">
         <v>104.062600256</v>
       </c>
@@ -27363,7 +27367,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="303" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A303">
         <v>58.041864812</v>
       </c>
@@ -27452,7 +27456,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="304" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A304">
         <v>28.031300128000002</v>
       </c>
@@ -27541,7 +27545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="305" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A305">
         <v>68.062600255999996</v>
       </c>
@@ -27630,7 +27634,7 @@
         <v>0.91483800109829772</v>
       </c>
     </row>
-    <row r="306" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A306">
         <v>68.062600255999996</v>
       </c>
@@ -27719,7 +27723,7 @@
         <v>0.69901903140956212</v>
       </c>
     </row>
-    <row r="307" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A307">
         <v>68.062600255999996</v>
       </c>
@@ -27808,7 +27812,7 @@
         <v>0.61435588108573902</v>
       </c>
     </row>
-    <row r="308" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A308">
         <v>68.062600255999996</v>
       </c>
@@ -27897,7 +27901,7 @@
         <v>0.54103711644110963</v>
       </c>
     </row>
-    <row r="309" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A309">
         <v>68.062600255999996</v>
       </c>
@@ -27986,7 +27990,7 @@
         <v>0.81466776496430549</v>
       </c>
     </row>
-    <row r="310" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A310">
         <v>68.062600255999996</v>
       </c>
@@ -28075,7 +28079,7 @@
         <v>0.58185517561503963</v>
       </c>
     </row>
-    <row r="311" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A311">
         <v>68.062600255999996</v>
       </c>
@@ -28164,7 +28168,7 @@
         <v>0.49052563550193901</v>
       </c>
     </row>
-    <row r="312" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A312">
         <v>68.062600255999996</v>
       </c>
@@ -28253,7 +28257,7 @@
         <v>0.4114337397829293</v>
       </c>
     </row>
-    <row r="313" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A313">
         <v>68.062600255999996</v>
       </c>
@@ -28342,7 +28346,7 @@
         <v>0.49426505583013008</v>
       </c>
     </row>
-    <row r="314" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A314">
         <v>68.062600255999996</v>
       </c>
@@ -28431,7 +28435,7 @@
         <v>0.35435092062509682</v>
       </c>
     </row>
-    <row r="315" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A315">
         <v>68.062600255999996</v>
       </c>
@@ -28520,7 +28524,7 @@
         <v>0.29946431136004598</v>
       </c>
     </row>
-    <row r="316" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A316">
         <v>68.062600255999996</v>
       </c>

</xml_diff>